<commit_message>
added v4 genex access creation, updated passwords
</commit_message>
<xml_diff>
--- a/New Employee Access Template.xlsx
+++ b/New Employee Access Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\PycharmProjects\AutoCreateAccesses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\PycharmProjects\AutoAccesses\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F601F092-E63A-4F4E-814A-F9C9B0BF41DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="14625" windowHeight="2295"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="New Employee" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>System Category</t>
   </si>
@@ -72,9 +73,6 @@
     <t>http://genex.billing.com.au/Module/Main/login.aspx</t>
   </si>
   <si>
-    <t>Genex (V4)</t>
-  </si>
-  <si>
     <t>Telebill</t>
   </si>
   <si>
@@ -114,12 +112,6 @@
     <t>http://ims2.buroserv.com.au/login.php</t>
   </si>
   <si>
-    <t>Alfresco</t>
-  </si>
-  <si>
-    <t>http://docs.planettel.com.au:8080/share/page/</t>
-  </si>
-  <si>
     <t>Isphone Porta</t>
   </si>
   <si>
@@ -217,12 +209,15 @@
   </si>
   <si>
     <t>3cx</t>
+  </si>
+  <si>
+    <t>Genex (Buroserv)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -408,7 +403,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -445,6 +440,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -459,17 +460,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -751,11 +755,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR278"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +791,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -800,7 +804,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
@@ -811,7 +815,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -822,7 +826,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
@@ -833,7 +837,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -844,7 +848,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
@@ -855,278 +859,274 @@
       </c>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21"/>
+      <c r="B12" s="7" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="21"/>
       <c r="B14" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="21"/>
       <c r="B15" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="A18" s="25"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="15"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="6" t="s">
-        <v>32</v>
-      </c>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="4"/>
       <c r="E19" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>35</v>
+      <c r="A20" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>40</v>
+      <c r="A23" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
+      <c r="A24" s="28"/>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="C25" s="18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="4" t="s">
+      <c r="D25" s="19"/>
+      <c r="E25" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C26" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="5" t="s">
+    </row>
+    <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="4" t="s">
+      <c r="C27" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="5" t="s">
+      <c r="C28" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="19"/>
+      <c r="E28" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="4" t="s">
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
+      <c r="A31" s="28"/>
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="6"/>
     </row>
     <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -1134,37 +1134,37 @@
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="26"/>
+        <v>57</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
       <c r="E33" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="26"/>
+        <v>62</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1423,17 +1423,16 @@
     <mergeCell ref="A23:A32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1"/>
-    <hyperlink ref="E6" r:id="rId2"/>
-    <hyperlink ref="E17" r:id="rId3" display="http://provisioning.buroserv.com.au/login.php"/>
-    <hyperlink ref="E18" r:id="rId4"/>
-    <hyperlink ref="E19" r:id="rId5"/>
-    <hyperlink ref="E23" r:id="rId6"/>
-    <hyperlink ref="E24" r:id="rId7"/>
-    <hyperlink ref="E28" r:id="rId8"/>
-    <hyperlink ref="E29" r:id="rId9"/>
-    <hyperlink ref="E30" r:id="rId10"/>
-    <hyperlink ref="E34" r:id="rId11"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E17" r:id="rId3" display="http://provisioning.buroserv.com.au/login.php" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E19" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E28" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E29" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
fixed password bug. added accessRemover. updated Template.
</commit_message>
<xml_diff>
--- a/New Employee Access Template.xlsx
+++ b/New Employee Access Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\PycharmProjects\AutoAccesses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F601F092-E63A-4F4E-814A-F9C9B0BF41DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C165C91-CB38-4628-8CBE-EF05D1E9F977}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -67,9 +67,6 @@
     <t>https://octane.telcoinabox.com/tiab/</t>
   </si>
   <si>
-    <t>Genex</t>
-  </si>
-  <si>
     <t>http://genex.billing.com.au/Module/Main/login.aspx</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>IMS2</t>
   </si>
   <si>
-    <t>http://ims2.buroserv.com.au/login.php</t>
-  </si>
-  <si>
     <t>Isphone Porta</t>
   </si>
   <si>
@@ -212,6 +206,12 @@
   </si>
   <si>
     <t>Genex (Buroserv)</t>
+  </si>
+  <si>
+    <t>Genex (V4)</t>
+  </si>
+  <si>
+    <t>http://ims.buroserv.com.au/login.php</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR278"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,18 +850,18 @@
     <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="21"/>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
       <c r="B9" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -870,93 +870,93 @@
     <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="21"/>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
       <c r="E17" s="6" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -969,42 +969,42 @@
     <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="4"/>
       <c r="E19" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1012,112 +1012,112 @@
     </row>
     <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28"/>
       <c r="B24" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28"/>
       <c r="B25" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D25" s="19"/>
       <c r="E25" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
       <c r="B27" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28"/>
       <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" s="19"/>
       <c r="E28" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28"/>
       <c r="B30" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28"/>
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
@@ -1126,7 +1126,7 @@
     <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29"/>
       <c r="B32" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
@@ -1134,34 +1134,34 @@
     </row>
     <row r="33" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C33" s="16"/>
       <c r="D33" s="17"/>
       <c r="E33" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
       <c r="E34" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
@@ -1425,14 +1425,13 @@
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E17" r:id="rId3" display="http://provisioning.buroserv.com.au/login.php" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E19" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E28" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E29" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E34" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E23" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E24" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E28" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E29" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E30" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E34" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>